<commit_message>
04.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/February/All Details/29.02.2020/MC Bank Statement Feb'2020.xlsx
+++ b/2020/February/All Details/29.02.2020/MC Bank Statement Feb'2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599"/>
   </bookViews>
   <sheets>
     <sheet name="Feb'2020" sheetId="7" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t xml:space="preserve">Salary </t>
+  </si>
+  <si>
+    <t>Nogod</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1738,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1747,7 +1750,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1770,14 +1773,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2081,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2945,15 +2948,25 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="60"/>
-      <c r="B47" s="66"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
+      <c r="B47" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="64">
+        <v>150000</v>
+      </c>
+      <c r="D47" s="135">
+        <v>150000</v>
+      </c>
       <c r="E47" s="95">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="2"/>
+      <c r="F47" s="136" t="s">
+        <v>53</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="H47" s="60"/>
     </row>
     <row r="48" spans="1:8">
@@ -3353,11 +3366,11 @@
       <c r="B83" s="72"/>
       <c r="C83" s="67">
         <f>SUM(C5:C72)</f>
-        <v>11728000</v>
+        <v>11878000</v>
       </c>
       <c r="D83" s="67">
         <f>SUM(D5:D77)</f>
-        <v>11725000</v>
+        <v>11875000</v>
       </c>
       <c r="E83" s="73">
         <f>E71+C83-D83</f>
@@ -3390,7 +3403,7 @@
   </sheetPr>
   <dimension ref="A1:AK222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>